<commit_message>
Note lec "Execution Contexts and The Call Stack"
</commit_message>
<xml_diff>
--- a/JavaScript-Course-Jonas-Schmedtmann/08-Behind-the-Scenes/Note.xlsx
+++ b/JavaScript-Course-Jonas-Schmedtmann/08-Behind-the-Scenes/Note.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desmonor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desmonor\Dropbox\learnToCode\Tech\JavaScript\Js-JavaScript-Course-Jonas-Schmedtmann\JavaScript-Course-Jonas-Schmedtmann\08-Behind-the-Scenes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6B1BEF-6730-4B9E-A8E8-22A30AA1AE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A279BB06-580A-4A03-924D-959A2E34A7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,10 +339,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -494,6 +494,226 @@
         <a:xfrm>
           <a:off x="14693153" y="3917576"/>
           <a:ext cx="7602071" cy="3469369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2277036</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>35860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>276673</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>118958</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCF3BB72-7FE7-4C09-8B88-C49B0A3E58E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11564471" y="10874189"/>
+          <a:ext cx="6462320" cy="2019475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>735106</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>8964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1475686</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>180485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0DE1ED2-0553-41C2-870F-CFF71102AD51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4491318" y="11277599"/>
+          <a:ext cx="6271803" cy="3398815"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>663388</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>125506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1434451</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>93043</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6AB3E4-380F-4686-A8C8-759206C484DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="15482047"/>
+          <a:ext cx="6302286" cy="2979678"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>663388</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1449692</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>74576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D4639AE-D96B-412F-8FD5-499B24A91DB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="18843811"/>
+          <a:ext cx="6317527" cy="1966130"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2411506</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>220626</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>26531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C90FE0-2510-4B31-8B0C-9190C79B780D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11698941" y="13554636"/>
+          <a:ext cx="6271803" cy="967824"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -770,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="F13:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -815,7 +1035,7 @@
       <c r="J14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -827,17 +1047,17 @@
         <v>10</v>
       </c>
       <c r="J15" s="4"/>
-      <c r="K15" s="8"/>
+      <c r="K15" s="9"/>
     </row>
     <row r="16" spans="6:11" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H16" s="5"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="8"/>
+      <c r="K16" s="9"/>
     </row>
     <row r="17" spans="8:11" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H17" s="5"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="8"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="8:11" ht="18" x14ac:dyDescent="0.3">
       <c r="H18" s="1" t="s">

</xml_diff>